<commit_message>
update gui and fixed single scan file
</commit_message>
<xml_diff>
--- a/all_macs/Known Mac address.xlsx
+++ b/all_macs/Known Mac address.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>Mac Address</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>TP-Link</t>
+  </si>
+  <si>
+    <t>FE-6F-C3-6C-0F-44</t>
+  </si>
+  <si>
+    <t>Nadine</t>
   </si>
 </sst>
 </file>
@@ -331,8 +337,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C62" totalsRowShown="0">
-  <autoFilter ref="A1:C62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C63" totalsRowShown="0">
+  <autoFilter ref="A1:C63"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Mac Address"/>
     <tableColumn id="2" name="PC Number" dataDxfId="1"/>
@@ -605,11 +611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,6 +1318,17 @@
         <v>68</v>
       </c>
     </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1 A56:A59">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>

</xml_diff>